<commit_message>
check values in test
</commit_message>
<xml_diff>
--- a/tests/data/duration.xlsx
+++ b/tests/data/duration.xlsx
@@ -275,7 +275,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -321,7 +321,7 @@
         <v>610</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" s="1"/>
     </row>

</xml_diff>